<commit_message>
TTR: only first million tokens are taken into account (for the amount of types, TTR is based on first million)
</commit_message>
<xml_diff>
--- a/freqs_sonar.xlsx
+++ b/freqs_sonar.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B33F7-046C-471F-9203-22D273A0C93F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA44019-4F22-4C5D-86E9-3F07D4977468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA863B94-EC8C-45BA-BB37-6BFA5EFAA374}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="doclength" sheetId="2" r:id="rId1"/>
+    <sheet name="TTR" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">doclength!$A$1:$D$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TTR!$F$5:$I$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>WORD LEVEL</t>
   </si>
@@ -124,14 +129,39 @@
 magazines</t>
   </si>
   <si>
-    <t>Typetokenratio</t>
+    <t> Group</t>
+  </si>
+  <si>
+    <t>#docs in group</t>
+  </si>
+  <si>
+    <t>#tokens in group</t>
+  </si>
+  <si>
+    <t>Average document length</t>
+  </si>
+  <si>
+    <t>Periodicals &amp; magazines</t>
+  </si>
+  <si>
+    <t>Texts for the visually impaired</t>
+  </si>
+  <si>
+    <t>Websites</t>
+  </si>
+  <si>
+    <t>Typetokenratio (of first 1 million words)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +175,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -252,7 +314,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,6 +352,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -575,11 +667,372 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA3D617-FE35-4177-9AB4-9626F1FE14E9}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14">
+        <v>139765</v>
+      </c>
+      <c r="C2" s="13">
+        <v>778</v>
+      </c>
+      <c r="D2" s="13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="14">
+        <v>26184781</v>
+      </c>
+      <c r="C3" s="13">
+        <v>507</v>
+      </c>
+      <c r="D3" s="14">
+        <v>51647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1213382</v>
+      </c>
+      <c r="C4" s="13">
+        <v>86</v>
+      </c>
+      <c r="D4" s="14">
+        <v>14109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14">
+        <v>11873434</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1304</v>
+      </c>
+      <c r="D5" s="14">
+        <v>9105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="14">
+        <v>57070554</v>
+      </c>
+      <c r="C6" s="14">
+        <v>702090</v>
+      </c>
+      <c r="D6" s="13">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14">
+        <v>8626248</v>
+      </c>
+      <c r="C7" s="14">
+        <v>18699</v>
+      </c>
+      <c r="D7" s="13">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="18">
+        <v>236099</v>
+      </c>
+      <c r="C8" s="17">
+        <v>12</v>
+      </c>
+      <c r="D8" s="18">
+        <v>19675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="14">
+        <v>10689681</v>
+      </c>
+      <c r="C9" s="14">
+        <v>7860</v>
+      </c>
+      <c r="D9" s="14">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="18">
+        <v>35446</v>
+      </c>
+      <c r="C10" s="17">
+        <v>9</v>
+      </c>
+      <c r="D10" s="18">
+        <v>3938</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="14">
+        <v>211669748</v>
+      </c>
+      <c r="C11" s="14">
+        <v>708600</v>
+      </c>
+      <c r="D11" s="13">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="14">
+        <v>93058924</v>
+      </c>
+      <c r="C12" s="14">
+        <v>176043</v>
+      </c>
+      <c r="D12" s="13">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="14">
+        <v>8711551</v>
+      </c>
+      <c r="C13" s="13">
+        <v>216</v>
+      </c>
+      <c r="D13" s="14">
+        <v>40331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="14">
+        <v>332795</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1053</v>
+      </c>
+      <c r="D14" s="13">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="18">
+        <v>314025</v>
+      </c>
+      <c r="C15" s="17">
+        <v>18</v>
+      </c>
+      <c r="D15" s="18">
+        <v>17446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2218223</v>
+      </c>
+      <c r="C16" s="17">
+        <v>81</v>
+      </c>
+      <c r="D16" s="18">
+        <v>27385</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14">
+        <v>723876</v>
+      </c>
+      <c r="C17" s="13">
+        <v>218</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="14">
+        <v>28209846</v>
+      </c>
+      <c r="C18" s="14">
+        <v>8368</v>
+      </c>
+      <c r="D18" s="14">
+        <v>3371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="14">
+        <v>448865</v>
+      </c>
+      <c r="C19" s="13">
+        <v>93</v>
+      </c>
+      <c r="D19" s="14">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="14">
+        <v>675082</v>
+      </c>
+      <c r="C20" s="13">
+        <v>943</v>
+      </c>
+      <c r="D20" s="13">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="14">
+        <v>23197211</v>
+      </c>
+      <c r="C21" s="13">
+        <v>602</v>
+      </c>
+      <c r="D21" s="14">
+        <v>38534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="14">
+        <v>3111589</v>
+      </c>
+      <c r="C22" s="13">
+        <v>956</v>
+      </c>
+      <c r="D22" s="14">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="14">
+        <v>23001184</v>
+      </c>
+      <c r="C23" s="14">
+        <v>124124</v>
+      </c>
+      <c r="D23" s="13">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="14">
+        <v>357947</v>
+      </c>
+      <c r="C24" s="13">
+        <v>188</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1904</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D24" xr:uid="{C74B051B-A32B-473A-8028-4A2F5950A8E0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
+      <sortCondition ref="A1:A24"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357E06D1-FE12-4135-A883-BBBB9B77ADEA}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,8 +1045,8 @@
     <col min="8" max="8" width="17" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="21.85546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="11.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -612,19 +1065,19 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -637,7 +1090,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="3" t="s">
@@ -650,383 +1103,731 @@
         <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="11">
         <v>139765</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="11">
         <v>18525</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="21">
+        <f>IF(B6&lt;1000000,C6/B6,C6/1000000)</f>
+        <v>0.13254391299681609</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="11"/>
+      <c r="G6" s="11">
+        <f>B6</f>
+        <v>139765</v>
+      </c>
+      <c r="H6" s="11">
+        <v>15716</v>
+      </c>
+      <c r="I6" s="26">
+        <f>IF(G6&lt;1000000,H6/G6,H6/1000000)</f>
+        <v>0.11244589131756878</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="11">
         <v>26184781</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="11">
         <v>37090</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="21">
+        <f>IF(B7&lt;1000000,C7/B7,C7/1000000)</f>
+        <v>3.7089999999999998E-2</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="G7" s="11">
+        <f>B7</f>
+        <v>26184781</v>
+      </c>
+      <c r="H7" s="11">
+        <v>26383</v>
+      </c>
+      <c r="I7" s="26">
+        <f>IF(G7&lt;1000000,H7/G7,H7/1000000)</f>
+        <v>2.6383E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="11">
         <v>1213382</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="11">
         <v>50400</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="21">
+        <f>IF(B8&lt;1000000,C8/B8,C8/1000000)</f>
+        <v>5.04E-2</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="G8" s="11">
+        <f>B8</f>
+        <v>1213382</v>
+      </c>
+      <c r="H8" s="11">
+        <v>42333</v>
+      </c>
+      <c r="I8" s="26">
+        <f>IF(G8&lt;1000000,H8/G8,H8/1000000)</f>
+        <v>4.2333000000000003E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="11">
         <v>11873434</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="11">
         <v>47974</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="21">
+        <f>IF(B9&lt;1000000,C9/B9,C9/1000000)</f>
+        <v>4.7974000000000003E-2</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="G9" s="11">
+        <f>B9</f>
+        <v>11873434</v>
+      </c>
+      <c r="H9" s="11">
+        <v>41974</v>
+      </c>
+      <c r="I9" s="26">
+        <f>IF(G9&lt;1000000,H9/G9,H9/1000000)</f>
+        <v>4.1973999999999997E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="11">
         <v>57070554</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="11">
         <v>64647</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="21">
+        <f>IF(B10&lt;1000000,C10/B10,C10/1000000)</f>
+        <v>6.4646999999999996E-2</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="G10" s="11">
+        <f>B10</f>
+        <v>57070554</v>
+      </c>
+      <c r="H10" s="11">
+        <v>54900</v>
+      </c>
+      <c r="I10" s="26">
+        <f>IF(G10&lt;1000000,H10/G10,H10/1000000)</f>
+        <v>5.4899999999999997E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="11">
         <v>8626248</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="11">
         <v>68054</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="21">
+        <f>IF(B11&lt;1000000,C11/B11,C11/1000000)</f>
+        <v>6.8054000000000003E-2</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="G11" s="11">
+        <f>B11</f>
+        <v>8626248</v>
+      </c>
+      <c r="H11" s="11">
+        <v>59169</v>
+      </c>
+      <c r="I11" s="26">
+        <f>IF(G11&lt;1000000,H11/G11,H11/1000000)</f>
+        <v>5.9168999999999999E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="25">
+        <v>236099</v>
+      </c>
+      <c r="C12" s="11">
+        <v>10397</v>
+      </c>
+      <c r="D12" s="21">
+        <f>IF(B12&lt;1000000,C12/B12,C12/1000000)</f>
+        <v>4.4036611760320879E-2</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="G12" s="11">
+        <f>B12</f>
+        <v>236099</v>
+      </c>
+      <c r="H12" s="11">
+        <v>8522</v>
+      </c>
+      <c r="I12" s="26">
+        <f>IF(G12&lt;1000000,H12/G12,H12/1000000)</f>
+        <v>3.6095027933197514E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="B13" s="11">
+        <v>10689681</v>
+      </c>
+      <c r="C13" s="11">
+        <v>34241</v>
+      </c>
+      <c r="D13" s="21">
+        <f>IF(B13&lt;1000000,C13/B13,C13/1000000)</f>
+        <v>3.4241000000000001E-2</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="G13" s="11">
+        <f>B13</f>
+        <v>10689681</v>
+      </c>
+      <c r="H13" s="11">
+        <v>31036</v>
+      </c>
+      <c r="I13" s="26">
+        <f>IF(G13&lt;1000000,H13/G13,H13/1000000)</f>
+        <v>3.1036000000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2">
-        <v>68054</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="11">
+        <v>35446</v>
+      </c>
+      <c r="C14" s="11">
         <v>4750</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="21">
+        <f>IF(B14&lt;1000000,C14/B14,C14/1000000)</f>
+        <v>0.13400665801500874</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="G14" s="11">
+        <f>B14</f>
+        <v>35446</v>
+      </c>
+      <c r="H14" s="11">
+        <v>3932</v>
+      </c>
+      <c r="I14" s="26">
+        <f>IF(G14&lt;1000000,H14/G14,H14/1000000)</f>
+        <v>0.11092930090842408</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="11">
+        <v>211669748</v>
+      </c>
+      <c r="C15" s="11">
+        <v>80021</v>
+      </c>
+      <c r="D15" s="21">
+        <f>IF(B15&lt;1000000,C15/B15,C15/1000000)</f>
+        <v>8.0020999999999995E-2</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="G15" s="11">
+        <f>B15</f>
+        <v>211669748</v>
+      </c>
+      <c r="H15" s="11">
+        <v>68765</v>
+      </c>
+      <c r="I15" s="26">
+        <f>IF(G15&lt;1000000,H15/G15,H15/1000000)</f>
+        <v>6.8765000000000007E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="19">
+        <v>93058924</v>
+      </c>
+      <c r="C16" s="11">
+        <v>83762</v>
+      </c>
+      <c r="D16" s="21">
+        <f>IF(B16&lt;1000000,C16/B16,C16/1000000)</f>
+        <v>8.3762000000000003E-2</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="11">
+        <f>B16</f>
+        <v>93058924</v>
+      </c>
+      <c r="H16" s="11">
+        <v>70858</v>
+      </c>
+      <c r="I16" s="26">
+        <f>IF(G16&lt;1000000,H16/G16,H16/1000000)</f>
+        <v>7.0858000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="19">
+        <v>8711551</v>
+      </c>
+      <c r="C17" s="11">
+        <v>33386</v>
+      </c>
+      <c r="D17" s="21">
+        <f>IF(B17&lt;1000000,C17/B17,C17/1000000)</f>
+        <v>3.3385999999999999E-2</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="11">
+        <f>B17</f>
+        <v>8711551</v>
+      </c>
+      <c r="H17" s="11">
+        <v>26151</v>
+      </c>
+      <c r="I17" s="26">
+        <f>IF(G17&lt;1000000,H17/G17,H17/1000000)</f>
+        <v>2.6151000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="11">
+        <v>332795</v>
+      </c>
+      <c r="C18" s="11">
+        <v>21200</v>
+      </c>
+      <c r="D18" s="21">
+        <f>IF(B18&lt;1000000,C18/B18,C18/1000000)</f>
+        <v>6.3702880151444582E-2</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="11">
+        <f>B18</f>
+        <v>332795</v>
+      </c>
+      <c r="H18" s="11">
+        <v>18155</v>
+      </c>
+      <c r="I18" s="26">
+        <f>IF(G18&lt;1000000,H18/G18,H18/1000000)</f>
+        <v>5.4553103261767752E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="20">
+        <v>314025</v>
+      </c>
+      <c r="C19" s="11">
+        <v>17707</v>
+      </c>
+      <c r="D19" s="21">
+        <f>IF(B19&lt;1000000,C19/B19,C19/1000000)</f>
+        <v>5.6387230316057642E-2</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="11">
+        <f>B19</f>
+        <v>314025</v>
+      </c>
+      <c r="H19" s="11">
+        <v>13985</v>
+      </c>
+      <c r="I19" s="26">
+        <f>IF(G19&lt;1000000,H19/G19,H19/1000000)</f>
+        <v>4.4534670806464456E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="20">
+        <v>2218223</v>
+      </c>
+      <c r="C20" s="11">
+        <v>44844</v>
+      </c>
+      <c r="D20" s="21">
+        <f>IF(B20&lt;1000000,C20/B20,C20/1000000)</f>
+        <v>4.4844000000000002E-2</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="11">
+        <f>B20</f>
+        <v>2218223</v>
+      </c>
+      <c r="H20" s="11">
+        <v>35824</v>
+      </c>
+      <c r="I20" s="26">
+        <f>IF(G20&lt;1000000,H20/G20,H20/1000000)</f>
+        <v>3.5824000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="19">
+        <v>723876</v>
+      </c>
+      <c r="C21" s="11">
+        <v>32917</v>
+      </c>
+      <c r="D21" s="21">
+        <f>IF(B21&lt;1000000,C21/B21,C21/1000000)</f>
+        <v>4.5473257850792127E-2</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="11">
+        <f>B21</f>
+        <v>723876</v>
+      </c>
+      <c r="H21" s="11">
+        <v>28569</v>
+      </c>
+      <c r="I21" s="26">
+        <f>IF(G21&lt;1000000,H21/G21,H21/1000000)</f>
+        <v>3.9466704242163024E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="B22" s="19">
+        <v>28209846</v>
+      </c>
+      <c r="C22" s="11">
+        <v>42304</v>
+      </c>
+      <c r="D22" s="21">
+        <f>IF(B22&lt;1000000,C22/B22,C22/1000000)</f>
+        <v>4.2304000000000001E-2</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="11">
+        <f>B22</f>
+        <v>28209846</v>
+      </c>
+      <c r="H22" s="11">
+        <v>33924</v>
+      </c>
+      <c r="I22" s="26">
+        <f>IF(G22&lt;1000000,H22/G22,H22/1000000)</f>
+        <v>3.3924000000000003E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="19">
+        <v>448865</v>
+      </c>
+      <c r="C23" s="11">
+        <v>29956</v>
+      </c>
+      <c r="D23" s="21">
+        <f>IF(B23&lt;1000000,C23/B23,C23/1000000)</f>
+        <v>6.6737214975549436E-2</v>
+      </c>
       <c r="E23" s="6"/>
       <c r="F23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G23" s="11">
+        <f>B23</f>
+        <v>448865</v>
+      </c>
+      <c r="H23" s="11">
+        <v>24050</v>
+      </c>
+      <c r="I23" s="26">
+        <f>IF(G23&lt;1000000,H23/G23,H23/1000000)</f>
+        <v>5.3579584062023101E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="19">
+        <v>675082</v>
+      </c>
+      <c r="C24" s="11">
+        <v>37624</v>
+      </c>
+      <c r="D24" s="21">
+        <f>IF(B24&lt;1000000,C24/B24,C24/1000000)</f>
+        <v>5.573248879395392E-2</v>
+      </c>
       <c r="E24" s="6"/>
       <c r="F24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="11">
+        <f>B24</f>
+        <v>675082</v>
+      </c>
+      <c r="H24" s="11">
+        <v>29562</v>
+      </c>
+      <c r="I24" s="26">
+        <f>IF(G24&lt;1000000,H24/G24,H24/1000000)</f>
+        <v>4.3790235852829727E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="19">
+        <v>23197211</v>
+      </c>
+      <c r="C25" s="11">
+        <v>81037</v>
+      </c>
+      <c r="D25" s="21">
+        <f>IF(B25&lt;1000000,C25/B25,C25/1000000)</f>
+        <v>8.1036999999999998E-2</v>
+      </c>
       <c r="E25" s="6"/>
       <c r="F25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="11">
+        <f>B25</f>
+        <v>23197211</v>
+      </c>
+      <c r="H25" s="11">
+        <v>73810</v>
+      </c>
+      <c r="I25" s="26">
+        <f>IF(G25&lt;1000000,H25/G25,H25/1000000)</f>
+        <v>7.3810000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B26" s="19">
+        <v>3111589</v>
+      </c>
+      <c r="C26" s="11">
+        <v>44722</v>
+      </c>
+      <c r="D26" s="21">
+        <f>IF(B26&lt;1000000,C26/B26,C26/1000000)</f>
+        <v>4.4721999999999998E-2</v>
+      </c>
       <c r="E26" s="6"/>
       <c r="F26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="11">
+        <f>B26</f>
+        <v>3111589</v>
+      </c>
+      <c r="H26" s="11">
+        <v>37183</v>
+      </c>
+      <c r="I26" s="26">
+        <f>IF(G26&lt;1000000,H26/G26,H26/1000000)</f>
+        <v>3.7183000000000001E-2</v>
+      </c>
+      <c r="K26" s="16"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="16"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="19">
+        <v>23001184</v>
+      </c>
+      <c r="C27" s="11">
+        <v>96842</v>
+      </c>
+      <c r="D27" s="21">
+        <f>IF(B27&lt;1000000,C27/B27,C27/1000000)</f>
+        <v>9.6841999999999998E-2</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="11">
+        <f>B27</f>
+        <v>23001184</v>
+      </c>
+      <c r="H27" s="11">
+        <v>87259</v>
+      </c>
+      <c r="I27" s="26">
+        <f>IF(G27&lt;1000000,H27/G27,H27/1000000)</f>
+        <v>8.7259000000000003E-2</v>
+      </c>
+      <c r="K27" s="16"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="19">
+        <v>357947</v>
+      </c>
+      <c r="C28" s="11">
+        <v>7732</v>
+      </c>
+      <c r="D28" s="21">
+        <f>IF(B28&lt;1000000,C28/B28,C28/1000000)</f>
+        <v>2.1600963271098794E-2</v>
+      </c>
       <c r="E28" s="6"/>
       <c r="F28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="G28" s="11">
+        <f>B28</f>
+        <v>357947</v>
+      </c>
+      <c r="H28" s="11">
+        <v>6338</v>
+      </c>
+      <c r="I28" s="26">
+        <f>IF(G28&lt;1000000,H28/G28,H28/1000000)</f>
+        <v>1.7706531972610469E-2</v>
+      </c>
+      <c r="K28" s="16"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="16"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K29" s="16"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
     </row>
   </sheetData>
+  <autoFilter ref="F5:I28" xr:uid="{38B989B1-9309-49D7-A98A-643F3C4ADCC4}"/>
   <mergeCells count="2">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F4:I4"/>

</xml_diff>

<commit_message>
added TTR for first million words of each collection
</commit_message>
<xml_diff>
--- a/freqs_sonar.xlsx
+++ b/freqs_sonar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA44019-4F22-4C5D-86E9-3F07D4977468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA785A44-7050-4F0A-932A-9C834F202FE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA863B94-EC8C-45BA-BB37-6BFA5EFAA374}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{DA863B94-EC8C-45BA-BB37-6BFA5EFAA374}"/>
   </bookViews>
   <sheets>
     <sheet name="doclength" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">doclength!$A$1:$D$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TTR!$F$5:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TTR!$A$5:$D$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>WORD LEVEL</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Typetokenratio (of first 1 million words)</t>
+  </si>
+  <si>
+    <t>high TTR</t>
+  </si>
+  <si>
+    <t>high degree of lexical variation</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +230,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,15 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -343,6 +347,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,8 +357,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -670,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA3D617-FE35-4177-9AB4-9626F1FE14E9}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -682,338 +696,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <v>139765</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="9">
         <v>778</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>26184781</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="9">
         <v>507</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <v>51647</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>1213382</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="9">
         <v>86</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <v>14109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>11873434</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>1304</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="10">
         <v>9105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="10">
         <v>57070554</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="10">
         <v>702090</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="9">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="10">
         <v>8626248</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="10">
         <v>18699</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="9">
         <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <v>236099</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>12</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>19675</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="10">
         <v>10689681</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="10">
         <v>7860</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="10">
         <v>1360</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <v>35446</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="13">
         <v>9</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <v>3938</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="10">
         <v>211669748</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="10">
         <v>708600</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="9">
         <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="10">
         <v>93058924</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="10">
         <v>176043</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="9">
         <v>529</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="10">
         <v>8711551</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>216</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="10">
         <v>40331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="10">
         <v>332795</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="10">
         <v>1053</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="9">
         <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="14">
         <v>314025</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="13">
         <v>18</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="14">
         <v>17446</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="14">
         <v>2218223</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="13">
         <v>81</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="14">
         <v>27385</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="10">
         <v>723876</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="9">
         <v>218</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="10">
         <v>3321</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="10">
         <v>28209846</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="10">
         <v>8368</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="10">
         <v>3371</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="10">
         <v>448865</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="9">
         <v>93</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="10">
         <v>4827</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="10">
         <v>675082</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="9">
         <v>943</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="9">
         <v>716</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="10">
         <v>23197211</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="9">
         <v>602</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="10">
         <v>38534</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="10">
         <v>3111589</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="9">
         <v>956</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="10">
         <v>3255</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="10">
         <v>23001184</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="10">
         <v>124124</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="9">
         <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="10">
         <v>357947</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="9">
         <v>188</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="10">
         <v>1904</v>
       </c>
     </row>
@@ -1029,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357E06D1-FE12-4135-A883-BBBB9B77ADEA}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,31 +1067,31 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="22" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1092,7 +1106,7 @@
       <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1108,711 +1122,712 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="11">
-        <v>139765</v>
-      </c>
-      <c r="C6" s="11">
-        <v>18525</v>
-      </c>
-      <c r="D6" s="21">
+        <v>25</v>
+      </c>
+      <c r="B6" s="15">
+        <v>357947</v>
+      </c>
+      <c r="C6" s="7">
+        <v>7732</v>
+      </c>
+      <c r="D6" s="17">
         <f>IF(B6&lt;1000000,C6/B6,C6/1000000)</f>
-        <v>0.13254391299681609</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>2.1600963271098794E-2</v>
+      </c>
+      <c r="E6" s="26"/>
       <c r="F6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="11">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7">
         <f>B6</f>
-        <v>139765</v>
-      </c>
-      <c r="H6" s="11">
-        <v>15716</v>
-      </c>
-      <c r="I6" s="26">
+        <v>357947</v>
+      </c>
+      <c r="H6" s="7">
+        <v>6338</v>
+      </c>
+      <c r="I6" s="18">
         <f>IF(G6&lt;1000000,H6/G6,H6/1000000)</f>
-        <v>0.11244589131756878</v>
+        <v>1.7706531972610469E-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="11">
-        <v>26184781</v>
-      </c>
-      <c r="C7" s="11">
-        <v>37090</v>
-      </c>
-      <c r="D7" s="21">
+        <v>15</v>
+      </c>
+      <c r="B7" s="15">
+        <v>8711551</v>
+      </c>
+      <c r="C7" s="7">
+        <v>33386</v>
+      </c>
+      <c r="D7" s="17">
         <f>IF(B7&lt;1000000,C7/B7,C7/1000000)</f>
-        <v>3.7089999999999998E-2</v>
-      </c>
-      <c r="E7" s="6"/>
+        <v>3.3385999999999999E-2</v>
+      </c>
+      <c r="E7" s="26"/>
       <c r="F7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="11">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7">
         <f>B7</f>
-        <v>26184781</v>
-      </c>
-      <c r="H7" s="11">
-        <v>26383</v>
-      </c>
-      <c r="I7" s="26">
+        <v>8711551</v>
+      </c>
+      <c r="H7" s="7">
+        <v>26151</v>
+      </c>
+      <c r="I7" s="18">
         <f>IF(G7&lt;1000000,H7/G7,H7/1000000)</f>
-        <v>2.6383E-2</v>
+        <v>2.6151000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="11">
-        <v>1213382</v>
-      </c>
-      <c r="C8" s="11">
-        <v>50400</v>
-      </c>
-      <c r="D8" s="21">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>10689681</v>
+      </c>
+      <c r="C8" s="7">
+        <v>34241</v>
+      </c>
+      <c r="D8" s="17">
         <f>IF(B8&lt;1000000,C8/B8,C8/1000000)</f>
-        <v>5.04E-2</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>3.4241000000000001E-2</v>
+      </c>
+      <c r="E8" s="26"/>
       <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="11">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7">
         <f>B8</f>
-        <v>1213382</v>
-      </c>
-      <c r="H8" s="11">
-        <v>42333</v>
-      </c>
-      <c r="I8" s="26">
+        <v>10689681</v>
+      </c>
+      <c r="H8" s="7">
+        <v>26383</v>
+      </c>
+      <c r="I8" s="18">
         <f>IF(G8&lt;1000000,H8/G8,H8/1000000)</f>
-        <v>4.2333000000000003E-2</v>
+        <v>2.6383E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="11">
-        <v>11873434</v>
-      </c>
-      <c r="C9" s="11">
-        <v>47974</v>
-      </c>
-      <c r="D9" s="21">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>26184781</v>
+      </c>
+      <c r="C9" s="7">
+        <v>37090</v>
+      </c>
+      <c r="D9" s="17">
         <f>IF(B9&lt;1000000,C9/B9,C9/1000000)</f>
-        <v>4.7974000000000003E-2</v>
-      </c>
-      <c r="E9" s="6"/>
+        <v>3.7089999999999998E-2</v>
+      </c>
+      <c r="E9" s="26"/>
       <c r="F9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="11">
+        <v>13</v>
+      </c>
+      <c r="G9" s="7">
         <f>B9</f>
-        <v>11873434</v>
-      </c>
-      <c r="H9" s="11">
-        <v>41974</v>
-      </c>
-      <c r="I9" s="26">
+        <v>26184781</v>
+      </c>
+      <c r="H9" s="7">
+        <v>31036</v>
+      </c>
+      <c r="I9" s="18">
         <f>IF(G9&lt;1000000,H9/G9,H9/1000000)</f>
-        <v>4.1973999999999997E-2</v>
+        <v>3.1036000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="11">
-        <v>57070554</v>
-      </c>
-      <c r="C10" s="11">
-        <v>64647</v>
-      </c>
-      <c r="D10" s="21">
+        <v>20</v>
+      </c>
+      <c r="B10" s="15">
+        <v>28209846</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42304</v>
+      </c>
+      <c r="D10" s="17">
         <f>IF(B10&lt;1000000,C10/B10,C10/1000000)</f>
-        <v>6.4646999999999996E-2</v>
-      </c>
-      <c r="E10" s="6"/>
+        <v>4.2304000000000001E-2</v>
+      </c>
+      <c r="E10" s="26"/>
       <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="11">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7">
         <f>B10</f>
-        <v>57070554</v>
-      </c>
-      <c r="H10" s="11">
-        <v>54900</v>
-      </c>
-      <c r="I10" s="26">
+        <v>28209846</v>
+      </c>
+      <c r="H10" s="7">
+        <v>33924</v>
+      </c>
+      <c r="I10" s="18">
         <f>IF(G10&lt;1000000,H10/G10,H10/1000000)</f>
-        <v>5.4899999999999997E-2</v>
+        <v>3.3924000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="11">
-        <v>8626248</v>
-      </c>
-      <c r="C11" s="11">
-        <v>68054</v>
-      </c>
-      <c r="D11" s="21">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <v>236099</v>
+      </c>
+      <c r="C11" s="7">
+        <v>10397</v>
+      </c>
+      <c r="D11" s="17">
         <f>IF(B11&lt;1000000,C11/B11,C11/1000000)</f>
-        <v>6.8054000000000003E-2</v>
-      </c>
-      <c r="E11" s="6"/>
+        <v>4.4036611760320879E-2</v>
+      </c>
+      <c r="E11" s="26"/>
       <c r="F11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="11">
+        <v>18</v>
+      </c>
+      <c r="G11" s="7">
         <f>B11</f>
-        <v>8626248</v>
-      </c>
-      <c r="H11" s="11">
-        <v>59169</v>
-      </c>
-      <c r="I11" s="26">
+        <v>236099</v>
+      </c>
+      <c r="H11" s="7">
+        <v>35824</v>
+      </c>
+      <c r="I11" s="18">
         <f>IF(G11&lt;1000000,H11/G11,H11/1000000)</f>
-        <v>5.9168999999999999E-2</v>
+        <v>0.15173295947886267</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="25">
-        <v>236099</v>
-      </c>
-      <c r="C12" s="11">
-        <v>10397</v>
-      </c>
-      <c r="D12" s="21">
+        <v>35</v>
+      </c>
+      <c r="B12" s="22">
+        <v>3111589</v>
+      </c>
+      <c r="C12" s="7">
+        <v>44722</v>
+      </c>
+      <c r="D12" s="17">
         <f>IF(B12&lt;1000000,C12/B12,C12/1000000)</f>
-        <v>4.4036611760320879E-2</v>
-      </c>
-      <c r="E12" s="6"/>
+        <v>4.4721999999999998E-2</v>
+      </c>
+      <c r="E12" s="26"/>
       <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="7">
         <f>B12</f>
-        <v>236099</v>
-      </c>
-      <c r="H12" s="11">
+        <v>3111589</v>
+      </c>
+      <c r="H12" s="7">
         <v>8522</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="18">
         <f>IF(G12&lt;1000000,H12/G12,H12/1000000)</f>
-        <v>3.6095027933197514E-2</v>
+        <v>8.5220000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="11">
-        <v>10689681</v>
-      </c>
-      <c r="C13" s="11">
-        <v>34241</v>
-      </c>
-      <c r="D13" s="21">
+        <v>18</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2218223</v>
+      </c>
+      <c r="C13" s="7">
+        <v>44844</v>
+      </c>
+      <c r="D13" s="17">
         <f>IF(B13&lt;1000000,C13/B13,C13/1000000)</f>
-        <v>3.4241000000000001E-2</v>
-      </c>
-      <c r="E13" s="6"/>
+        <v>4.4844000000000002E-2</v>
+      </c>
+      <c r="E13" s="26"/>
       <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="11">
+        <v>23</v>
+      </c>
+      <c r="G13" s="7">
         <f>B13</f>
-        <v>10689681</v>
-      </c>
-      <c r="H13" s="11">
-        <v>31036</v>
-      </c>
-      <c r="I13" s="26">
+        <v>2218223</v>
+      </c>
+      <c r="H13" s="7">
+        <v>37183</v>
+      </c>
+      <c r="I13" s="18">
         <f>IF(G13&lt;1000000,H13/G13,H13/1000000)</f>
-        <v>3.1036000000000001E-2</v>
+        <v>3.7183000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11">
-        <v>35446</v>
-      </c>
-      <c r="C14" s="11">
-        <v>4750</v>
-      </c>
-      <c r="D14" s="21">
+        <v>19</v>
+      </c>
+      <c r="B14" s="15">
+        <v>723876</v>
+      </c>
+      <c r="C14" s="7">
+        <v>32917</v>
+      </c>
+      <c r="D14" s="17">
         <f>IF(B14&lt;1000000,C14/B14,C14/1000000)</f>
-        <v>0.13400665801500874</v>
-      </c>
-      <c r="E14" s="6"/>
+        <v>4.5473257850792127E-2</v>
+      </c>
+      <c r="E14" s="26"/>
       <c r="F14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="11">
+        <v>19</v>
+      </c>
+      <c r="G14" s="7">
         <f>B14</f>
-        <v>35446</v>
-      </c>
-      <c r="H14" s="11">
-        <v>3932</v>
-      </c>
-      <c r="I14" s="26">
+        <v>723876</v>
+      </c>
+      <c r="H14" s="7">
+        <v>28569</v>
+      </c>
+      <c r="I14" s="18">
         <f>IF(G14&lt;1000000,H14/G14,H14/1000000)</f>
-        <v>0.11092930090842408</v>
+        <v>3.9466704242163024E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11">
-        <v>211669748</v>
-      </c>
-      <c r="C15" s="11">
-        <v>80021</v>
-      </c>
-      <c r="D15" s="21">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <v>11873434</v>
+      </c>
+      <c r="C15" s="7">
+        <v>47974</v>
+      </c>
+      <c r="D15" s="17">
         <f>IF(B15&lt;1000000,C15/B15,C15/1000000)</f>
-        <v>8.0020999999999995E-2</v>
-      </c>
-      <c r="E15" s="6"/>
+        <v>4.7974000000000003E-2</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="11">
+        <v>6</v>
+      </c>
+      <c r="G15" s="7">
         <f>B15</f>
-        <v>211669748</v>
-      </c>
-      <c r="H15" s="11">
-        <v>68765</v>
-      </c>
-      <c r="I15" s="26">
+        <v>11873434</v>
+      </c>
+      <c r="H15" s="7">
+        <v>41974</v>
+      </c>
+      <c r="I15" s="18">
         <f>IF(G15&lt;1000000,H15/G15,H15/1000000)</f>
-        <v>6.8765000000000007E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="19">
-        <v>93058924</v>
-      </c>
-      <c r="C16" s="11">
-        <v>83762</v>
-      </c>
-      <c r="D16" s="21">
+        <v>4.1973999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1213382</v>
+      </c>
+      <c r="C16" s="7">
+        <v>50400</v>
+      </c>
+      <c r="D16" s="17">
         <f>IF(B16&lt;1000000,C16/B16,C16/1000000)</f>
-        <v>8.3762000000000003E-2</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="11">
+        <v>5.04E-2</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="7">
         <f>B16</f>
-        <v>93058924</v>
-      </c>
-      <c r="H16" s="11">
-        <v>70858</v>
-      </c>
-      <c r="I16" s="26">
+        <v>1213382</v>
+      </c>
+      <c r="H16" s="7">
+        <v>42333</v>
+      </c>
+      <c r="I16" s="18">
         <f>IF(G16&lt;1000000,H16/G16,H16/1000000)</f>
-        <v>7.0858000000000004E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="19">
-        <v>8711551</v>
-      </c>
-      <c r="C17" s="11">
-        <v>33386</v>
-      </c>
-      <c r="D17" s="21">
+        <v>4.2333000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="15">
+        <v>675082</v>
+      </c>
+      <c r="C17" s="7">
+        <v>37624</v>
+      </c>
+      <c r="D17" s="17">
         <f>IF(B17&lt;1000000,C17/B17,C17/1000000)</f>
-        <v>3.3385999999999999E-2</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="11">
+        <v>5.573248879395392E-2</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="7">
         <f>B17</f>
-        <v>8711551</v>
-      </c>
-      <c r="H17" s="11">
-        <v>26151</v>
-      </c>
-      <c r="I17" s="26">
+        <v>675082</v>
+      </c>
+      <c r="H17" s="7">
+        <v>29562</v>
+      </c>
+      <c r="I17" s="18">
         <f>IF(G17&lt;1000000,H17/G17,H17/1000000)</f>
-        <v>2.6151000000000001E-2</v>
+        <v>4.3790235852829727E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="11">
-        <v>332795</v>
-      </c>
-      <c r="C18" s="11">
-        <v>21200</v>
-      </c>
-      <c r="D18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16">
+        <v>314025</v>
+      </c>
+      <c r="C18" s="7">
+        <v>17707</v>
+      </c>
+      <c r="D18" s="17">
         <f>IF(B18&lt;1000000,C18/B18,C18/1000000)</f>
-        <v>6.3702880151444582E-2</v>
-      </c>
-      <c r="E18" s="6"/>
+        <v>5.6387230316057642E-2</v>
+      </c>
+      <c r="E18" s="26"/>
       <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="11">
+        <v>17</v>
+      </c>
+      <c r="G18" s="7">
         <f>B18</f>
-        <v>332795</v>
-      </c>
-      <c r="H18" s="11">
-        <v>18155</v>
-      </c>
-      <c r="I18" s="26">
+        <v>314025</v>
+      </c>
+      <c r="H18" s="7">
+        <v>13985</v>
+      </c>
+      <c r="I18" s="18">
         <f>IF(G18&lt;1000000,H18/G18,H18/1000000)</f>
-        <v>5.4553103261767752E-2</v>
+        <v>4.4534670806464456E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="20">
-        <v>314025</v>
-      </c>
-      <c r="C19" s="11">
-        <v>17707</v>
-      </c>
-      <c r="D19" s="21">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7">
+        <v>332795</v>
+      </c>
+      <c r="C19" s="7">
+        <v>21200</v>
+      </c>
+      <c r="D19" s="17">
         <f>IF(B19&lt;1000000,C19/B19,C19/1000000)</f>
-        <v>5.6387230316057642E-2</v>
-      </c>
-      <c r="E19" s="6"/>
+        <v>6.3702880151444582E-2</v>
+      </c>
+      <c r="E19" s="26"/>
       <c r="F19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="11">
+        <v>21</v>
+      </c>
+      <c r="G19" s="7">
         <f>B19</f>
-        <v>314025</v>
-      </c>
-      <c r="H19" s="11">
-        <v>13985</v>
-      </c>
-      <c r="I19" s="26">
+        <v>332795</v>
+      </c>
+      <c r="H19" s="7">
+        <v>24050</v>
+      </c>
+      <c r="I19" s="18">
         <f>IF(G19&lt;1000000,H19/G19,H19/1000000)</f>
-        <v>4.4534670806464456E-2</v>
+        <v>7.2266710737841619E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="20">
-        <v>2218223</v>
-      </c>
-      <c r="C20" s="11">
-        <v>44844</v>
-      </c>
-      <c r="D20" s="21">
+        <v>11</v>
+      </c>
+      <c r="B20" s="7">
+        <v>57070554</v>
+      </c>
+      <c r="C20" s="7">
+        <v>64647</v>
+      </c>
+      <c r="D20" s="17">
         <f>IF(B20&lt;1000000,C20/B20,C20/1000000)</f>
-        <v>4.4844000000000002E-2</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>6.4646999999999996E-2</v>
+      </c>
+      <c r="E20" s="26"/>
       <c r="F20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="11">
+        <v>16</v>
+      </c>
+      <c r="G20" s="7">
         <f>B20</f>
-        <v>2218223</v>
-      </c>
-      <c r="H20" s="11">
-        <v>35824</v>
-      </c>
-      <c r="I20" s="26">
+        <v>57070554</v>
+      </c>
+      <c r="H20" s="7">
+        <v>18155</v>
+      </c>
+      <c r="I20" s="18">
         <f>IF(G20&lt;1000000,H20/G20,H20/1000000)</f>
-        <v>3.5824000000000002E-2</v>
+        <v>1.8155000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="19">
-        <v>723876</v>
-      </c>
-      <c r="C21" s="11">
-        <v>32917</v>
-      </c>
-      <c r="D21" s="21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="15">
+        <v>448865</v>
+      </c>
+      <c r="C21" s="7">
+        <v>29956</v>
+      </c>
+      <c r="D21" s="17">
         <f>IF(B21&lt;1000000,C21/B21,C21/1000000)</f>
-        <v>4.5473257850792127E-2</v>
-      </c>
-      <c r="E21" s="6"/>
+        <v>6.6737214975549436E-2</v>
+      </c>
+      <c r="E21" s="26"/>
       <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="11">
+        <v>11</v>
+      </c>
+      <c r="G21" s="7">
         <f>B21</f>
-        <v>723876</v>
-      </c>
-      <c r="H21" s="11">
-        <v>28569</v>
-      </c>
-      <c r="I21" s="26">
+        <v>448865</v>
+      </c>
+      <c r="H21" s="7">
+        <v>54900</v>
+      </c>
+      <c r="I21" s="18">
         <f>IF(G21&lt;1000000,H21/G21,H21/1000000)</f>
-        <v>3.9466704242163024E-2</v>
+        <v>0.12230848918939993</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="19">
-        <v>28209846</v>
-      </c>
-      <c r="C22" s="11">
-        <v>42304</v>
-      </c>
-      <c r="D22" s="21">
+        <v>7</v>
+      </c>
+      <c r="B22" s="7">
+        <v>8626248</v>
+      </c>
+      <c r="C22" s="7">
+        <v>68054</v>
+      </c>
+      <c r="D22" s="17">
         <f>IF(B22&lt;1000000,C22/B22,C22/1000000)</f>
-        <v>4.2304000000000001E-2</v>
-      </c>
-      <c r="E22" s="6"/>
+        <v>6.8054000000000003E-2</v>
+      </c>
+      <c r="E22" s="26"/>
       <c r="F22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="11">
+        <v>7</v>
+      </c>
+      <c r="G22" s="7">
         <f>B22</f>
-        <v>28209846</v>
-      </c>
-      <c r="H22" s="11">
-        <v>33924</v>
-      </c>
-      <c r="I22" s="26">
+        <v>8626248</v>
+      </c>
+      <c r="H22" s="7">
+        <v>59169</v>
+      </c>
+      <c r="I22" s="18">
         <f>IF(G22&lt;1000000,H22/G22,H22/1000000)</f>
-        <v>3.3924000000000003E-2</v>
+        <v>5.9168999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="19">
-        <v>448865</v>
-      </c>
-      <c r="C23" s="11">
-        <v>29956</v>
-      </c>
-      <c r="D23" s="21">
+        <v>14</v>
+      </c>
+      <c r="B23" s="7">
+        <v>211669748</v>
+      </c>
+      <c r="C23" s="7">
+        <v>80021</v>
+      </c>
+      <c r="D23" s="17">
         <f>IF(B23&lt;1000000,C23/B23,C23/1000000)</f>
-        <v>6.6737214975549436E-2</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>8.0020999999999995E-2</v>
+      </c>
+      <c r="E23" s="26"/>
       <c r="F23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="11">
+        <v>14</v>
+      </c>
+      <c r="G23" s="7">
         <f>B23</f>
-        <v>448865</v>
-      </c>
-      <c r="H23" s="11">
-        <v>24050</v>
-      </c>
-      <c r="I23" s="26">
+        <v>211669748</v>
+      </c>
+      <c r="H23" s="7">
+        <v>68765</v>
+      </c>
+      <c r="I23" s="18">
         <f>IF(G23&lt;1000000,H23/G23,H23/1000000)</f>
-        <v>5.3579584062023101E-2</v>
+        <v>6.8765000000000007E-2</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="19">
-        <v>675082</v>
-      </c>
-      <c r="C24" s="11">
-        <v>37624</v>
-      </c>
-      <c r="D24" s="21">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="15">
+        <v>23197211</v>
+      </c>
+      <c r="C24" s="7">
+        <v>81037</v>
+      </c>
+      <c r="D24" s="17">
         <f>IF(B24&lt;1000000,C24/B24,C24/1000000)</f>
-        <v>5.573248879395392E-2</v>
-      </c>
-      <c r="E24" s="6"/>
+        <v>8.1036999999999998E-2</v>
+      </c>
+      <c r="E24" s="26"/>
       <c r="F24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="11">
+        <v>28</v>
+      </c>
+      <c r="G24" s="7">
         <f>B24</f>
-        <v>675082</v>
-      </c>
-      <c r="H24" s="11">
-        <v>29562</v>
-      </c>
-      <c r="I24" s="26">
+        <v>23197211</v>
+      </c>
+      <c r="H24" s="7">
+        <v>70858</v>
+      </c>
+      <c r="I24" s="18">
         <f>IF(G24&lt;1000000,H24/G24,H24/1000000)</f>
-        <v>4.3790235852829727E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="19">
-        <v>23197211</v>
-      </c>
-      <c r="C25" s="11">
-        <v>81037</v>
-      </c>
-      <c r="D25" s="21">
+        <v>7.0858000000000004E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="15">
+        <v>93058924</v>
+      </c>
+      <c r="C25" s="7">
+        <v>83762</v>
+      </c>
+      <c r="D25" s="17">
         <f>IF(B25&lt;1000000,C25/B25,C25/1000000)</f>
-        <v>8.1036999999999998E-2</v>
-      </c>
-      <c r="E25" s="6"/>
+        <v>8.3762000000000003E-2</v>
+      </c>
+      <c r="E25" s="26"/>
       <c r="F25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="7">
         <f>B25</f>
-        <v>23197211</v>
-      </c>
-      <c r="H25" s="11">
+        <v>93058924</v>
+      </c>
+      <c r="H25" s="7">
         <v>73810</v>
       </c>
-      <c r="I25" s="26">
+      <c r="I25" s="18">
         <f>IF(G25&lt;1000000,H25/G25,H25/1000000)</f>
         <v>7.3810000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="19">
-        <v>3111589</v>
-      </c>
-      <c r="C26" s="11">
-        <v>44722</v>
-      </c>
-      <c r="D26" s="21">
+        <v>24</v>
+      </c>
+      <c r="B26" s="15">
+        <v>23001184</v>
+      </c>
+      <c r="C26" s="7">
+        <v>96842</v>
+      </c>
+      <c r="D26" s="17">
         <f>IF(B26&lt;1000000,C26/B26,C26/1000000)</f>
-        <v>4.4721999999999998E-2</v>
-      </c>
-      <c r="E26" s="6"/>
+        <v>9.6841999999999998E-2</v>
+      </c>
+      <c r="E26" s="26"/>
       <c r="F26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="11">
+        <v>24</v>
+      </c>
+      <c r="G26" s="7">
         <f>B26</f>
-        <v>3111589</v>
-      </c>
-      <c r="H26" s="11">
-        <v>37183</v>
-      </c>
-      <c r="I26" s="26">
+        <v>23001184</v>
+      </c>
+      <c r="H26" s="7">
+        <v>87259</v>
+      </c>
+      <c r="I26" s="18">
         <f>IF(G26&lt;1000000,H26/G26,H26/1000000)</f>
-        <v>3.7183000000000001E-2</v>
-      </c>
-      <c r="K26" s="16"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="16"/>
+        <v>8.7259000000000003E-2</v>
+      </c>
+      <c r="K26" s="12"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="19">
-        <v>23001184</v>
-      </c>
-      <c r="C27" s="11">
-        <v>96842</v>
-      </c>
-      <c r="D27" s="21">
+        <v>2</v>
+      </c>
+      <c r="B27" s="7">
+        <v>139765</v>
+      </c>
+      <c r="C27" s="7">
+        <v>18525</v>
+      </c>
+      <c r="D27" s="17">
         <f>IF(B27&lt;1000000,C27/B27,C27/1000000)</f>
-        <v>9.6841999999999998E-2</v>
-      </c>
-      <c r="E27" s="6"/>
+        <v>0.13254391299681609</v>
+      </c>
+      <c r="E27" s="26"/>
       <c r="F27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
         <f>B27</f>
-        <v>23001184</v>
-      </c>
-      <c r="H27" s="11">
-        <v>87259</v>
-      </c>
-      <c r="I27" s="26">
+        <v>139765</v>
+      </c>
+      <c r="H27" s="7">
+        <v>3932</v>
+      </c>
+      <c r="I27" s="18">
         <f>IF(G27&lt;1000000,H27/G27,H27/1000000)</f>
-        <v>8.7259000000000003E-2</v>
-      </c>
-      <c r="K27" s="16"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="16"/>
+        <v>2.8132937430687226E-2</v>
+      </c>
+      <c r="K27" s="12"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="19">
-        <v>357947</v>
-      </c>
-      <c r="C28" s="11">
-        <v>7732</v>
-      </c>
-      <c r="D28" s="21">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7">
+        <v>35446</v>
+      </c>
+      <c r="C28" s="7">
+        <v>4750</v>
+      </c>
+      <c r="D28" s="17">
         <f>IF(B28&lt;1000000,C28/B28,C28/1000000)</f>
-        <v>2.1600963271098794E-2</v>
-      </c>
-      <c r="E28" s="6"/>
+        <v>0.13400665801500874</v>
+      </c>
+      <c r="E28" s="26"/>
       <c r="F28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="11">
+        <v>2</v>
+      </c>
+      <c r="G28" s="7">
         <f>B28</f>
-        <v>357947</v>
-      </c>
-      <c r="H28" s="11">
-        <v>6338</v>
-      </c>
-      <c r="I28" s="26">
+        <v>35446</v>
+      </c>
+      <c r="H28" s="7">
+        <v>15716</v>
+      </c>
+      <c r="I28" s="18">
         <f>IF(G28&lt;1000000,H28/G28,H28/1000000)</f>
-        <v>1.7706531972610469E-2</v>
-      </c>
-      <c r="K28" s="16"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="16"/>
+        <v>0.44337866049765839</v>
+      </c>
+      <c r="K28" s="12"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K29" s="16"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="16"/>
+      <c r="E29" s="23"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="12"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K30"/>
@@ -1826,8 +1841,20 @@
       <c r="M31"/>
       <c r="N31"/>
     </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="F5:I28" xr:uid="{38B989B1-9309-49D7-A98A-643F3C4ADCC4}"/>
+  <autoFilter ref="A5:D28" xr:uid="{1914272F-10C9-4FD1-B1B8-D43CBAB71269}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:D28">
+      <sortCondition ref="D5:D28"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F4:I4"/>

</xml_diff>